<commit_message>
Updated Schematic and Readme
</commit_message>
<xml_diff>
--- a/rover/core/science/Schematic.xlsx
+++ b/rover/core/science/Schematic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Circuit" sheetId="2" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
   <si>
     <t>Array Format</t>
   </si>
@@ -261,6 +261,51 @@
   </si>
   <si>
     <t>http://www.co2meters.com/Documentation/AppNotes/AN102-K30-Sensor-Arduino-I2C.pdf</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Arduino Vin</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Arduino Analog A2</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Arduino requires 7V to 24V external power supply</t>
+  </si>
+  <si>
+    <t>sensors/Decagon5TE_EC</t>
+  </si>
+  <si>
+    <t>sensors/Decagon5TE_VWC</t>
+  </si>
+  <si>
+    <t>sensors/GUVAS12SD</t>
+  </si>
+  <si>
+    <t>sensors/MPL3115A2</t>
+  </si>
+  <si>
+    <t>sensors/MLX90614_Ambient</t>
+  </si>
+  <si>
+    <t>sensors/MLX90614_Object</t>
+  </si>
+  <si>
+    <t>sensors/DHT11</t>
+  </si>
+  <si>
+    <t>sensors/K30</t>
+  </si>
+  <si>
+    <t>sensors/Anemometer</t>
   </si>
 </sst>
 </file>
@@ -360,7 +405,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -376,6 +421,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -671,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:P30"/>
+  <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -983,6 +1030,37 @@
         <v>46</v>
       </c>
     </row>
+    <row r="31" spans="2:16" ht="15.75" customHeight="1"/>
+    <row r="32" spans="2:16">
+      <c r="B32" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
@@ -991,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1002,15 +1080,16 @@
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1023,8 +1102,11 @@
       <c r="D4" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1037,8 +1119,11 @@
       <c r="D5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1052,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1066,7 +1151,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1080,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1093,8 +1178,11 @@
       <c r="D9" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -1107,8 +1195,11 @@
       <c r="D10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1121,8 +1212,11 @@
       <c r="D11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -1136,7 +1230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -1150,7 +1244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
         <v>10</v>
       </c>
@@ -1163,8 +1257,11 @@
       <c r="D14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
         <v>11</v>
       </c>
@@ -1177,8 +1274,11 @@
       <c r="D15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
         <v>12</v>
       </c>
@@ -1192,7 +1292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
         <v>13</v>
       </c>
@@ -1206,7 +1306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
         <v>14</v>
       </c>
@@ -1219,8 +1319,11 @@
       <c r="D18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
         <v>15</v>
       </c>
@@ -1232,6 +1335,26 @@
       </c>
       <c r="D19" t="s">
         <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>